<commit_message>
WIP XL Table support
</commit_message>
<xml_diff>
--- a/test/data/test-table-advance.xlsx
+++ b/test/data/test-table-advance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobc/Data/Code/aoba/aobaJSXL/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ED56B1-F6C5-134B-A0E8-2D44B64C2DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280EA9C0-596F-D741-AAC2-69E54281EF85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{C4356EEB-D4B1-1746-BA0A-A1EF7529741D}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{C4356EEB-D4B1-1746-BA0A-A1EF7529741D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96FC0B3A-DFCD-B547-891E-04F26CA6B570}" name="Table1" displayName="Table1" ref="A1:D5" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96FC0B3A-DFCD-B547-891E-04F26CA6B570}" name="TableEmployee" displayName="TableEmployee" ref="A1:D5" totalsRowShown="0">
   <autoFilter ref="A1:D5" xr:uid="{96FC0B3A-DFCD-B547-891E-04F26CA6B570}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{57993C06-B5DA-184E-8DA2-8ABF6C9BE641}" name="Id"/>
@@ -237,7 +237,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9596F5F3-51F1-004D-8961-FF4982AEC878}" name="Table2" displayName="Table2" ref="C9:E15" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9596F5F3-51F1-004D-8961-FF4982AEC878}" name="CityTable" displayName="CityTable" ref="C9:E15" totalsRowShown="0">
   <autoFilter ref="C9:E15" xr:uid="{9596F5F3-51F1-004D-8961-FF4982AEC878}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9F1D62E6-79DB-6640-92F1-D0F57990F06B}" name="CityId"/>
@@ -249,7 +249,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4D886F8F-D48F-FD4F-8D23-0BA3BEDF3662}" name="Table3" displayName="Table3" ref="I9:K17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4D886F8F-D48F-FD4F-8D23-0BA3BEDF3662}" name="VehicleTable" displayName="VehicleTable" ref="I9:K17" totalsRowShown="0">
   <autoFilter ref="I9:K17" xr:uid="{4D886F8F-D48F-FD4F-8D23-0BA3BEDF3662}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{2351C1B5-E525-8940-BB22-634841D5D2C8}" name="VehicleId"/>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B40CC7F9-1D5E-BC46-A06E-9E08712A9F31}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -668,9 +668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{406BB9B6-4BA4-1047-87DA-FEF575B9B612}">
   <dimension ref="C9:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>